<commit_message>
[+] info xlsx init [+] changed writer
</commit_message>
<xml_diff>
--- a/output/1.xlsx
+++ b/output/1.xlsx
@@ -371,22 +371,22 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Почта преподавателя</t>
+          <t>Название предмета</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Телефон преподавателя</t>
+          <t>Время с</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Название предмета</t>
+          <t>Время по</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Время с</t>
+          <t>Ссылка</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">

</xml_diff>